<commit_message>
ajout de nouveaux enregistrements
</commit_message>
<xml_diff>
--- a/data_labeled_wtj.xlsx
+++ b/data_labeled_wtj.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d595cbf690a07aed/Documents/Capitalyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{1BF085DF-0EBD-4B03-AD17-7A9C5B2F8EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCFBE05B-9EEE-4651-A6DC-3D9D03F7FCFC}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="8_{1BF085DF-0EBD-4B03-AD17-7A9C5B2F8EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{797093F1-04DE-4ED7-AF16-16F4C55BB208}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D79B2E10-14FD-46E5-84BA-125D9DC4AD2D}"/>
+    <workbookView xWindow="-2175" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D79B2E10-14FD-46E5-84BA-125D9DC4AD2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="131">
   <si>
     <t>from</t>
   </si>
@@ -473,6 +473,365 @@
   </si>
   <si>
     <t>til-8cb7e0a1d5bfbd8cdd74c1b5@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour,
+Nous vous remercions pour l'intérêt que vous portez à notre entreprise.
+Après étude de votre candidature, nous sommes au regret de vous annoncer que nous ne pouvons pas lui donner une suite favorable. En effet, votre profil ne correspond pas aux attentes que nous avons sur ce poste.
+Nous vous souhaitons une bonne continuation dans vos recherches.
+Cordialement,
+L'équipe The Information Lab
+Pour répondre, envoyez un email à :
+til-8cb7e0a1d5bfbd8cdd74c1b5@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>The Information Lab - Votre candidature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Hello Julien,
+Un grand merci pour votre candidature et pour l’intérêt que vous portez à ARMIS. Nous sommes toujours à la recherche de nouveaux talents pour rejoindre notre aventure!
+Cependant, après étude de votre candidature et malgré toutes ses qualités, nous avons décidé de ne pas la sélectionner pour la prochaine étape. Nous restons à votre disposition si vous souhaitez un retour plus personnalisé concernant le refus.
+Nous vous souhaitons beaucoup de réussite dans votre recherche et surtout n’hésitez pas à visiter notre page ARMIS pour plus d’informations et pour être au courant de nos dernières offres !
+A très bientôt,
+Massara NEMLIN
+HR Project Manager
+Pour répondre, envoyez un email à :
+armis-4af39d21f998eef6834b672c@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Candidature Solutions Engineer - (CDI) - H/F - Paris - ARMIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci de l'intérêt que vous portez au poste de Data engineer chez Edumapper et pour votre enthousiasme pour notre projet.
+Après avoir examiné votre profil, nous avons décidé de ne pas donner suite à votre candidature pour le moment. Cette décision ne remet pas en question la qualité de votre parcours, mais nous recherchons un profil qui correspond plus précisément aux besoins actuels de l'entreprise.
+N'hésitez pas à visiter notre site carrière régulièrement, nous y publions souvent de nouvelles offres : https://edumapper.notion.site/Rejoindre-Edumapper-c8400b9ea3d34a2eaf69fbd32d42ad16
+Par ailleurs, nous vous proposons de conserver votre CV pendant 2 an(s) dans notre CVthèque afin de vous recontacter si nous ouvrons un poste correspondant à votre profil. Si vous ne le souhaitez pas, vous pouvez nous en informer par retour d'email.
+Nous vous souhaitons beaucoup de succès dans votre recherche d'emploi.
+A très bientôt,
+Aminata Diagne
+Pour répondre, envoyez un email à :
+eduma-0bd59bcb959c559cc98a726f@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Votre candidature pour le poste de Data engineer</t>
+  </si>
+  <si>
+    <t>eduma-0bd59bcb959c559cc98a726f@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci pour votre candidature, je suis ravi que vous vous intéressiez à IKA !
+Je souhaite vous informer que nous avons choisi de poursuivre le recrutement avec d'autres candidats.
+Cela ne remet pas en cause la qualité de votre profil, mais simplement un meilleur alignement avec nos besoins actuels.
+Je vous souhaite le meilleur pour la suite de votre recherche et votre parcours professionnel.
+Cordialement,
+L'équipe IKA
+Pour répondre, envoyez un email à :
+ika-dd37fa6ff07649e9e50cc6b4@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Votre candidature au poste de Data base engineer SQL et PLSQL (H/F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Nous vous remercions de l’intérêt que vous avez manifesté pour le poste d’Analytics Engineer / Data Engineer F/H chez Urgo Medical (Paris, Île-de-France).
+Nous tenons à vous informer que ce poste a été pourvu. Nous vous remercions sincèrement du temps que vous avez consacré à votre candidature et de l’intérêt porté à Urgo Medical.
+Cordialement,
+L’équipe Urgo Medical
+Pour répondre, envoyez un email à :
+urgo-bb2eb99d52f5310b7d51ebc5@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Votre candidature – Urgo Medical</t>
+  </si>
+  <si>
+    <t>urgo-bb2eb99d52f5310b7d51ebc5@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci pour votre candidature mais malheureusement celle-ci n'a pas été retenue pour le poste de "Data Engineering - CDI".
+Nous tenions tout de même à vous remercier de votre intérêt pour Polynom et pour les échanges que nous avons eus. Nous vous souhaitons également beaucoup de réussite dans vos recherches.
+A très bientôt,
+Mélissa Sid Larbi
+Pour répondre, envoyez un email à :
+polyn-731bb1643c9e7ea55a710061@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t>Votre candidature pour le poste de Data Engineering - CDI - Polynom</t>
+  </si>
+  <si>
+    <t>polyn-731bb1643c9e7ea55a710061@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci pour ta candidature et ton intérêt pour Arkhn. Malheureusement nous ne pourrons pas donner suite à ta candidature au poste de Junior Analytics Engineer.
+Nous avons reçu beaucoup d'excellents profils et nous avons donc fait un choix en conséquence.
+Bonne continuation dans ta recherche,
+Cordialement,
+L'équipe Arkhn
+Pour répondre, envoyez un email à :
+arkhn-41acf78d451d889ced56fa85@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Candidature pour le poste de Junior Analytics Engineer</t>
+  </si>
+  <si>
+    <t>arkhn-41acf78d451d889ced56fa85@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Malheureusement, votre candidature n'a pas été retenue pour le poste de "Data engineer"
+Nous avons privilégié des profils ayant une expérience plus en adéquation avec nos besoins.
+N'hésitez pas à visiter notre site carrière régulièrement, nous y publions souvent de nouvelles offres.
+A très bientôt,
+Anne-Lise LEBAYLE
+Pour répondre, envoyez un email à :
+garan-589902ac5e3466ab77fb0699@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Bonjour Julien, votre candidature pour le poste de Data engineer</t>
+  </si>
+  <si>
+    <t>garan-589902ac5e3466ab77fb0699@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci pour votre candidature, je suis ravi que vous vous intéressiez à IKA !
+Je souhaite vous informer que nous avons choisi de poursuivre le recrutement avec d'autres candidats.
+Cela ne remet pas en cause la qualité de votre profil, mais simplement un meilleur alignement avec nos besoins actuels.
+Je vous souhaite le meilleur pour la suite de votre recherche et votre parcours professionnel.
+Cordialement,
+L'équipe IKA
+Pour répondre, envoyez un email à :
+ika-ce4fc691fe9b10013a3ff47d@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Votre candidature au poste de Ingénieur Data PL/SQL - Confirmé (H/F)</t>
+  </si>
+  <si>
+    <t>ika-ce4fc691fe9b10013a3ff47d@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Nous vous remercions pour l’intérêt que vous portez à la Clinique des Champs-Élysées et pour votre candidature au poste de Data Analyst.
+Nous souhaitions vous informer que le processus de recrutement pour ce poste est actuellement suspendu. Nous ne pouvons donc pas poursuivre l’étude des candidatures pour le moment.
+Nous conserverons toutefois votre dossier et ne manquerons pas de revenir vers vous dès que le recrutement reprendra ou si une opportunité similaire se présente.
+Nous vous remercions pour votre compréhension et pour l’intérêt que vous portez à notre établissement.
+Nous vous souhaitons une excellente fin de journée ainsi qu’une très bonne continuation dans vos recherches.
+Bien cordialement,
+L'équipe RH.
+Pour répondre, envoyez un email à :
+cdce-c2ccad3f1e83fc02de79e3af@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Candidature Clinique des Champs-Elysées</t>
+  </si>
+  <si>
+    <t>cdce-c2ccad3f1e83fc02de79e3af@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci encore pour ta candidature 🙌
+Nous aimerions planifier un premier échange de 15 minutes par visio afin de mieux comprendre ton parcours et tes envies, et de te présenter Yomoni plus en détail.
+📅 Pour choisir le créneau qui t’arrange le mieux, il te suffit de cliquer ici :
+👉 https://calendly.com/benjamin-levain-h9e/entretien-data-engineer
+À très vite,
+Benjamin Levain
+Pour répondre, envoyez un email à :
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>On fait connaissance ? ☎️</t>
+  </si>
+  <si>
+    <t>↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci pour le temps que tu as pris pour échanger avec nous mercredi 🙌
+Nous avons apprécié ton profil, ton état d'esprit et ta volonté de toujours vouloir apprendre davantage et construire des solutions. C'est pourquoi nous attendons pas plus longtemps pour te faire avancer dans le processus.
+👉 Prochaine étape : le cas pratique ✏️
+Comme évoqué au téléphone , il a lieu en présentiel dans nos locaux au 6 rue Auber , 75008 , Paris et dure 2h30 sur place ( 1h15 de préparation et 1h d'échanges).
+Tu recevras 10 minutes avant toutes les infos nécessaires pour le réaliser.
+Quelles seraient tes disponibilités la semaine prochaine ? Je te donne des créneaux
+Lundi 24 novembre à 14h , 15h ou 16h et donc jusqu'à 16h/16H30 si 14h , ...)
+Mardi 25 novembre à 16h ( et donc jusqu'à 18h/18H30)
+Mercredi 26 novembre à 16h ( et donc jusqu'à 18h/18H30)
+Si aucune date ne te convient hésite pas à m'en proposer d'autres mais on aimerait te voir cette semaine dans la mesure du possible
+On a hâte de continuer ce parcours avec toi 🚀
+À très vite,
+Benjamin Levain
+Yomoni
+Pour répondre, envoyez un email à :
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+↥ Répondre au dessus de cette ligne ↥
+Hello Julien ,
+C'est parfait c'est noté pour mercredi 16h. tu as dû recevoir une
+invitation avec l'adresse.
+Et oui si possible, viens avec ton ordinateur et installe un IDE et jupyter
+notebook si pas déjà fait.
+Et si tu peux arriver 10 minutes avant ce serait parfait. Je viendrai te
+chercher en bas dans le hall.
+Hésite pas si tu as des questions d'ici la.
+Très bon weekend,
+Benjamin
+On Fri, Nov 21, 2025 at 1:47 PM Jo &lt;
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co&gt; wrote:
+Pour répondre, envoyez un email à :
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t>↥ Répondre au dessus de cette ligne ↥
+Hello Julien,
+Tu peux m'envoyer un message directement au 0613364965 si tu préfères.
+A tout à l'heure.
+Benjamin
+On Wed, Nov 26, 2025 at 10:05 AM Jo &lt;
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co&gt; wrote:
+Pour répondre, envoyez un email à :
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci encore pour le temps que tu as consacré à échanger avec nous au sujet du poste de Data Engineer - CDI - Paris, ainsi que pour ta disponibilité lors de nos différents entretiens. Nous avons beaucoup apprécié apprendre à mieux te connaître et discuter avec toi de ton expérience et de tes motivations.
+Après réflexion et échanges au sein de l’équipe, nous avons pris la décision de ne pas poursuivre le processus de recrutement pour ce poste. Ce choix tient aux besoins spécifiques que nous devons couvrir aujourd’hui.
+Si tu souhaites obtenir plus de précisions sur cette décision, n’hésite pas à me le faire savoir, je serai ravie d’en discuter avec toi.
+Nous te remercions sincèrement pour ton implication et l’intérêt porté à Yomoni, et te souhaitons beaucoup de réussite dans la suite de tes projets professionnels.
+Bien à toi,
+Benjamin Levain
+Yomoni
+Pour répondre, envoyez un email à :
+yomon-017c613ae004832bb0f1afe3@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Retour suite à nos entretiens – Candidature Data Engineer - CDI - Paris</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci beaucoup de ton intérêt pour la position de Data fullstack chez Ekie.
+Malheureusement nous continuerons avec un autre candidat sur ce poste.
+Ce n'est jamais évident de choisir, et la compétition était rude sur ce poste.
+Nous te souhaitons bonne chance dans la suite de tes recherches. Restons en contact, la vie professionnelle est longue et réserve souvent de belles surprises.
+Bien à toi,
+L'Equipe Ekie
+Pour répondre, envoyez un email à :
+ekie-b6a779a688631411de447401@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Merci pour ta candidature chez Ekie</t>
+  </si>
+  <si>
+    <t>ekie-b6a779a688631411de447401@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Malheureusement, nous avons décidé de ne pas donner suite à votre candidature pour le poste de "Consultant·e Analytics/Data Engineer - DBT Snowflake (F/H)" car nous avons préféré privilégier un profil plus en adéquation avec notre besoin.
+Nous vous remercions sincèrement de l'intérêt que vous avez montré pour Actinvision et vous souhaitons d'aboutir dans vos recherches.
+N'hésitez pas à visiter notre site carrière régulièrement, nous y publions souvent de nouvelles offres.
+A très bientôt,
+L'équipe ACTINVISION
+Pour répondre, envoyez un email à :
+actin-070ca1635bd2da63236f4eb8@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Votre candidature pour le poste de Consultant·e Analytics/Data Engineer - DBT Snowflake (F/H)</t>
+  </si>
+  <si>
+    <t>actin-070ca1635bd2da63236f4eb8@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Reply above this line ↥
+Bonjour Julien,
+Nous vous remercions sincèrement pour l'intérêt que vous avez porté à notre entreprise et pour le temps consacré à votre candidature au poste de Senior Data Engineer (Python / SQL) - (M/F).
+Après une analyse attentive de votre profil, nous avons le regret de vous informer que nous ne donnerons pas suite à votre candidature.
+Cette décision ne remet pas en question la qualité de votre profil, qui pourrait tout à fait correspondre à d'autres opportunités que nous pourrions proposer à l'avenir.
+Nous vous souhaitons une bonne continuation dans vos projets professionnels.
+Cordialement,
+L'équipe Talent Acquisition de TCS France
+To reply, send an email to:
+tcst-054dca9017801b0260f6619b@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>tcst-054dca9017801b0260f6619b@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t>Julien Ohana x Tata Consultancy Services France : Retour de candidature Senior Data Engineer (Python / SQL) - (M/F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Malheureusement, nous avons décidé de ne pas donner suite à votre candidature pour le poste de "CONSULTANT.E SNOWFLAKE - DATA ENGINEER (F/H)" car nous avons préféré privilégier un profil plus en adéquation avec notre besoin.
+Nous vous remercions sincèrement de l'intérêt que vous avez montré pour Actinvision et vous souhaitons d'aboutir dans vos recherches.
+N'hésitez pas à visiter notre site carrière régulièrement, nous y publions souvent de nouvelles offres.
+A très bientôt,
+L'équipe ACTINVISION
+Pour répondre, envoyez un email à :
+actin-d42b5f3b645bfc3f7dd0afc1@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Votre candidature pour le poste de CONSULTANT.E SNOWFLAKE - DATA ENGINEER (F/H)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Merci beaucoup de ton intérêt pour la position de Data fullstack chez Ekie.
+Malheureusement nous continuerons avec un autre candidat sur ce poste.
+Ce n'est jamais évident de choisir, et la compétition était rude sur ce poste.
+Nous te souhaitons bonne chance dans la suite de tes recherches. Restons en contact, la vie professionnelle est longue et réserve souvent de belles surprises.
+Bien à toi,
+L'Equipe Ekie
+Pour répondre, envoyez un email à :
+ekie-f478adfc16502cefc04d24e7@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ekie-f478adfc16502cefc04d24e7@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Malgré l'intérêt de votre parcours, votre candidature n'a malheureusement pas été retenue car vos dates ne correspondent pas à ce que nous cherchons.
+Nous vous remercions néanmoins pour l'intérêt que vous portez à Craft AI et nous vous souhaitons bonne chance dans vos recherches.
+Cordialement,
+L'équipe Craft AI
+Pour répondre, envoyez un email à :
+ca-ccd633d8df3969a4a4af6853@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Candidature pour le poste de Stagiaire Développeur Backend chez Craft AI
+Boîte de réception</t>
+  </si>
+  <si>
+    <t>ca-ccd633d8df3969a4a4af6853@candidates.welcomekit.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ↥ Répondre au dessus de cette ligne ↥
+Bonjour Julien,
+Nous avons bien reçu votre candidature pour le poste de Candidatures spontanées et nous vous remercions pour tout l'intérêt que vous portez à Craft AI. Nous l'étudions avec attention et revenons vers vous dans les plus brefs délais si votre candidature est retenue.
+Devant l'affluence des candidatures, nous ne pouvons malheureusement pas répondre à tous les candidats donc si nous ne sommes pas revenus vers vous d'ici une quinzaine de jours, vous pouvez considérer que votre candidature n'a pas été retenue.
+A très bientôt,
+L'équipe Craft AI
+Pour répondre, envoyez un email à :
+ca-ccd633d8df3969a4a4af6853@candidates.welcomekit.co </t>
+  </si>
+  <si>
+    <t>Julien, candidature bien reçue pour Candidatures spontanées
+Boîte de réception</t>
   </si>
 </sst>
 </file>
@@ -520,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -529,6 +888,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -545,6 +907,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -864,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229A1AD2-5D76-49BA-B460-29A4C6155A68}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,9 +1680,417 @@
         <v>78</v>
       </c>
       <c r="D26" s="3">
-        <v>41147.568749999999</v>
+        <v>45895.568749999999</v>
       </c>
       <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45895.584722222222</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45897.375</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45898.65902777778</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45898.757638888892</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45901.68472222222</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45904.380555555559</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45908.443749999999</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45909.388888888891</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45937.461111111108</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45933.587500000001</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45985.371527777781</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="345.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45986.68472222222</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45975.731944444444</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45982.467361111114</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45983.775590277779</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45987.557650462964</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="360" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45992.617997685185</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45993.669548611113</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45995.612291666665</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45995.650254629632</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45996.371840277781</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D48" s="3">
+        <v>46006.666666666664</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="216" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="3">
+        <v>44714.433854166666</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="3">
+        <v>44700.851388888892</v>
+      </c>
+      <c r="E50">
         <v>1</v>
       </c>
     </row>
@@ -1347,8 +2121,32 @@
     <hyperlink ref="C24" r:id="rId23" xr:uid="{E3CD0C5F-B540-408E-A895-63D56C6750FC}"/>
     <hyperlink ref="C25" r:id="rId24" xr:uid="{2FF1CC79-599E-4AD7-8AB9-78D91E8EF07F}"/>
     <hyperlink ref="C26" r:id="rId25" xr:uid="{BBF53380-98EB-4CBD-ADE8-C1625979E3F9}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{7508C181-2906-439C-AEB8-E5FC4F355190}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{E18C2147-B9A8-4A51-AB3D-5636A322443E}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{98BF227C-EF1A-49BF-872A-4963C0FE333A}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{DB120867-B931-46AD-A579-725AF1460E62}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{E8DC7B35-2FFF-402E-BB89-B3F01F747392}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{72E58D2B-101A-4F85-BB50-29E954485F99}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{953F4A6C-C484-4C73-BB11-A9F8AA5B0735}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{2C70B6E8-E94A-4E19-95A2-0056C178E096}"/>
+    <hyperlink ref="C35" r:id="rId34" xr:uid="{6AE9BE6A-70D1-4356-80C1-171F4FAA196A}"/>
+    <hyperlink ref="C36" r:id="rId35" xr:uid="{D1FFAD3D-ADEB-4CA1-A961-D4C336A9C398}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{33B8B34D-E9C7-4C79-B0FF-0A70C447EBC6}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{4676BAE0-D674-45C4-A803-33EE19E56890}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{3973C013-3724-4A96-989B-E5EF8282126A}"/>
+    <hyperlink ref="C40" r:id="rId39" xr:uid="{E052C4CF-6B20-43B6-8CC3-81A78750F2D7}"/>
+    <hyperlink ref="C41" r:id="rId40" xr:uid="{03C31394-6B6C-4EAF-A937-D0D06DB95ACF}"/>
+    <hyperlink ref="C42" r:id="rId41" xr:uid="{C61878AC-51DD-483A-B770-D969B3BC1B33}"/>
+    <hyperlink ref="C43" r:id="rId42" xr:uid="{5E71AD65-331B-45D1-A4D4-8E444AD2AE16}"/>
+    <hyperlink ref="C44" r:id="rId43" xr:uid="{186195F2-8087-422E-A255-F1FD22DBEEC7}"/>
+    <hyperlink ref="C45" r:id="rId44" xr:uid="{9D92D75B-911C-492F-A683-1EA2FD5E2DE4}"/>
+    <hyperlink ref="C46" r:id="rId45" xr:uid="{81687014-E873-4E23-BEC2-0E68684E17FD}"/>
+    <hyperlink ref="C47" r:id="rId46" xr:uid="{B692ECE1-BF3C-49AA-BE3E-AF767C9D0883}"/>
+    <hyperlink ref="C48" r:id="rId47" xr:uid="{571AE1CB-ECC1-415D-98D0-9F936A566E81}"/>
+    <hyperlink ref="C49" r:id="rId48" xr:uid="{E2116975-E3D1-4735-B315-80BA983BB56B}"/>
+    <hyperlink ref="C50" r:id="rId49" xr:uid="{AB16E994-C863-471E-B393-F319AE6081E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
création d'un dataset inspiré de l'original by Chat GPT
</commit_message>
<xml_diff>
--- a/data_labeled_wtj.xlsx
+++ b/data_labeled_wtj.xlsx
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{229A1AD2-5D76-49BA-B460-29A4C6155A68}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>